<commit_message>
checking debugs and aesthetics
</commit_message>
<xml_diff>
--- a/Tasks_Examples.xlsx
+++ b/Tasks_Examples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/hossaina3745_masseyhigh_school_nz/Documents/2025 TCCOM/Recipe costs (assesment)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="691" documentId="8_{3E261E29-A1DC-4AC7-9AE9-7BE6C2A75354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{312DF900-A3AB-478C-AFFE-E114EE51F12D}"/>
+  <xr:revisionPtr revIDLastSave="794" documentId="8_{3E261E29-A1DC-4AC7-9AE9-7BE6C2A75354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33EAB61F-5969-4D04-B87F-11EA7D39A59B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8355E7AF-B006-48C4-BF9B-25D6A2537B13}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Servings</t>
   </si>
@@ -95,10 +95,43 @@
     </r>
   </si>
   <si>
-    <t>Flour</t>
-  </si>
-  <si>
-    <t>Sugar</t>
+    <t>Noodle</t>
+  </si>
+  <si>
+    <t>Ramen</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>Mushroom</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>Nori</t>
+  </si>
+  <si>
+    <t>Menma</t>
+  </si>
+  <si>
+    <t>Soy Sauce</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>Beef Stock</t>
+  </si>
+  <si>
+    <t>Total price</t>
   </si>
 </sst>
 </file>
@@ -108,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +180,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,8 +243,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -362,11 +414,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,6 +455,9 @@
     <xf numFmtId="8" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -406,6 +470,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,9 +480,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFE5E5"/>
       <color rgb="FFFFB3B3"/>
       <color rgb="FFFE6666"/>
-      <color rgb="FFFFE5E5"/>
       <color rgb="FFFFCDCD"/>
     </mruColors>
   </colors>
@@ -732,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53989F0C-4682-48E5-86E1-4253CFB56C21}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,17 +809,21 @@
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="22"/>
+      <c r="C1" s="34" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -762,35 +832,35 @@
       <c r="B2" s="23">
         <v>20</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:13" ht="26.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="E4" s="30" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="E4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -814,201 +884,256 @@
       <c r="H5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>150</v>
+        <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="14">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F6" s="15">
-        <v>1500</v>
+        <v>2.4</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H6" s="24">
         <f>E6/F6*A6</f>
-        <v>0.5</v>
-      </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
+        <v>20</v>
+      </c>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="16">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F7" s="17">
-        <v>2500</v>
+        <v>4</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H7" s="25">
         <f t="shared" ref="H7:H12" si="0">E7/F7*A7</f>
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
+        <v>40</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="E8" s="18"/>
+        <v>17</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="18">
+        <v>20</v>
+      </c>
       <c r="F8" s="19">
-        <v>1</v>
-      </c>
-      <c r="G8" s="19"/>
+        <v>2</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="H8" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
+        <v>16</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="E9" s="16"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="16">
+        <v>48</v>
+      </c>
       <c r="F9" s="17">
-        <v>1</v>
-      </c>
-      <c r="G9" s="17"/>
+        <v>10</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="H9" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
+        <v>38.4</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <v>1</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="E10" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="18">
+        <v>15</v>
+      </c>
       <c r="F10" s="19">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
+        <v>12.5</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <v>1</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="E11" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="16">
+        <v>6.8</v>
+      </c>
       <c r="F11" s="17">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
+        <v>6.7999999999999989</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="E12" s="20"/>
+      <c r="C12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="20">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="F12" s="21">
+        <v>500</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="21"/>
       <c r="H12" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G14" s="3" t="s">
+        <v>2.64</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <v>500</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="29">
+        <v>4.7</v>
+      </c>
+      <c r="F13" s="28">
+        <v>1</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="25">
+        <f>E13/2</f>
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="35">
+        <f>SUM(E6:E13)</f>
+        <v>162.9</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H17" s="24">
         <f>SUM(H6:H13)</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="F16" s="28" t="s">
+        <v>138.69</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="6:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="F19" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="26">
-        <f>H14/B2</f>
-        <v>3.4999999999999996E-2</v>
+      <c r="G19" s="31"/>
+      <c r="H19" s="26">
+        <f>H17/B2</f>
+        <v>6.9344999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="J2:M12"/>
-    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F19:G19"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="E4:H4"/>
   </mergeCells>

</xml_diff>